<commit_message>
housing model first year restauration calc
</commit_message>
<xml_diff>
--- a/input/hyperparameter.xlsx
+++ b/input/hyperparameter.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t xml:space="preserve">parameter</t>
   </si>
@@ -28,16 +28,34 @@
     <t xml:space="preserve">value</t>
   </si>
   <si>
+    <t xml:space="preserve">description</t>
+  </si>
+  <si>
     <t xml:space="preserve">bev_variant</t>
   </si>
   <si>
     <t xml:space="preserve">BEV-VARIANTE-03</t>
   </si>
   <si>
+    <t xml:space="preserve">choose the population variant from input file</t>
+  </si>
+  <si>
     <t xml:space="preserve">scenario</t>
   </si>
   <si>
     <t xml:space="preserve">all</t>
+  </si>
+  <si>
+    <t xml:space="preserve">choose scenario(s), comma spereated. Or choose all</t>
+  </si>
+  <si>
+    <t xml:space="preserve">restauration_building_type bias</t>
+  </si>
+  <si>
+    <t xml:space="preserve">no</t>
+  </si>
+  <si>
+    <t xml:space="preserve">choose how building types are affected by restauration: Either from the number of buildings (no)  or from the bias given in input file </t>
   </si>
 </sst>
 </file>
@@ -145,15 +163,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="26.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="55.02"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -163,21 +183,41 @@
       <c r="B1" s="0" t="s">
         <v>1</v>
       </c>
+      <c r="C1" s="0" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>5</v>
+        <v>7</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
restoration still buggy #1
</commit_message>
<xml_diff>
--- a/input/hyperparameter.xlsx
+++ b/input/hyperparameter.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t xml:space="preserve">parameter</t>
   </si>
@@ -43,7 +43,7 @@
     <t xml:space="preserve">scenario</t>
   </si>
   <si>
-    <t xml:space="preserve">all</t>
+    <t xml:space="preserve">soe</t>
   </si>
   <si>
     <t xml:space="preserve">choose scenario(s), comma spereated. Or choose all</t>
@@ -56,6 +56,15 @@
   </si>
   <si>
     <t xml:space="preserve">choose how building types are affected by restauration: Either from the number of buildings (no)  or from the bias given in input file </t>
+  </si>
+  <si>
+    <t xml:space="preserve">second_amb_restauration</t>
+  </si>
+  <si>
+    <t xml:space="preserve">yes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">yes or no. If yes, use restauration potential to restaurate ambitiously</t>
   </si>
 </sst>
 </file>
@@ -163,13 +172,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="212" zoomScaleNormal="212" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="26.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.7"/>
@@ -218,6 +227,17 @@
       </c>
       <c r="C4" s="0" t="s">
         <v>11</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added/finished new building and years
</commit_message>
<xml_diff>
--- a/input/hyperparameter.xlsx
+++ b/input/hyperparameter.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
   <si>
     <t xml:space="preserve">parameter</t>
   </si>
@@ -59,9 +59,6 @@
   </si>
   <si>
     <t xml:space="preserve">second_amb_restauration</t>
-  </si>
-  <si>
-    <t xml:space="preserve">yes</t>
   </si>
   <si>
     <t xml:space="preserve">yes or no. If yes, use restauration potential to restaurate ambitiously</t>
@@ -175,10 +172,10 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="212" zoomScaleNormal="212" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="26.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.7"/>
@@ -234,16 +231,16 @@
         <v>12</v>
       </c>
       <c r="B5" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="0" t="s">
         <v>13</v>
-      </c>
-      <c r="C5" s="0" t="s">
-        <v>14</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>

</xml_diff>